<commit_message>
many updates for many codes
I should be better doing these things with GitHub
</commit_message>
<xml_diff>
--- a/tables/summary_analyses.xlsx
+++ b/tables/summary_analyses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danmarti/Documents/MRC_postdoc/My_projects/Ecoli_metabolic_modelling/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB0B83-124B-6641-B561-FA80B37C21C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E3A818-6B2C-2F4C-B0D7-8307046E4AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{5F2FD370-ECF8-1648-BF24-94D6FCBB5462}"/>
   </bookViews>
@@ -444,7 +444,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,7 +539,7 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>21892</v>
+        <v>21083</v>
       </c>
       <c r="D6">
         <v>27876</v>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>5984</v>
+        <v>6793</v>
       </c>
       <c r="D12">
         <v>27876</v>

</xml_diff>